<commit_message>
Changed the tool statues to numbers
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2514D9D-C87E-064D-AD32-6F67580CF3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FE4AA-6CF1-964F-94D2-B8DFB383DE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
   <si>
     <t>I000240</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Main Office</t>
   </si>
   <si>
-    <t>Disabled</t>
-  </si>
-  <si>
     <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230322_141545-49E5A919-CDBF-4044-F465-E7F77739F08F.jpg</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
   </si>
   <si>
     <t>2.5</t>
-  </si>
-  <si>
-    <t>In Maintenance</t>
   </si>
   <si>
     <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/663889/image/20230919_152336-ED3ADFCF-DCC4-C14B-605D-D9E3CEE9426B.jpg</t>
@@ -760,7 +754,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,67 +783,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -869,10 +863,10 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -880,64 +874,64 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
         <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" t="s">
-        <v>10</v>
-      </c>
       <c r="R2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -945,11 +939,11 @@
       <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
-        <v>39</v>
+      <c r="J3">
+        <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
         <v>4</v>
@@ -958,64 +952,64 @@
         <v>4</v>
       </c>
       <c r="N3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="R3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="L4" t="s">
         <v>4</v>
       </c>
@@ -1023,64 +1017,64 @@
         <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O4" t="s">
         <v>3</v>
       </c>
       <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" t="s">
-        <v>10</v>
-      </c>
       <c r="R4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="L5" t="s">
         <v>4</v>
       </c>
@@ -1088,63 +1082,63 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O5" t="s">
         <v>3</v>
       </c>
       <c r="P5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" t="s">
-        <v>10</v>
-      </c>
       <c r="R5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
+        <v>57</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
@@ -1153,64 +1147,64 @@
         <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O6" t="s">
         <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="R6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S6" t="s">
-        <v>11</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="L7" t="s">
         <v>4</v>
       </c>
@@ -1218,129 +1212,129 @@
         <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O7" t="s">
         <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q7" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="R7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S7" t="s">
-        <v>11</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="M8" t="s">
         <v>4</v>
       </c>
       <c r="N8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O8" t="s">
         <v>3</v>
       </c>
       <c r="P8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" t="s">
         <v>80</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="U8" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="R8" t="s">
-        <v>11</v>
-      </c>
-      <c r="S8" t="s">
-        <v>11</v>
-      </c>
-      <c r="T8" t="s">
-        <v>82</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="L9" t="s">
         <v>4</v>
       </c>
@@ -1348,64 +1342,64 @@
         <v>4</v>
       </c>
       <c r="N9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O9" t="s">
         <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q9" t="s">
+        <v>87</v>
+      </c>
+      <c r="R9" t="s">
+        <v>88</v>
+      </c>
+      <c r="S9" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" t="s">
         <v>89</v>
       </c>
-      <c r="R9" t="s">
+      <c r="U9" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="S9" t="s">
-        <v>11</v>
-      </c>
-      <c r="T9" t="s">
-        <v>91</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>94</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="L10" t="s">
         <v>4</v>
       </c>
@@ -1413,64 +1407,64 @@
         <v>4</v>
       </c>
       <c r="N10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O10" t="s">
         <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q10" t="s">
+        <v>96</v>
+      </c>
+      <c r="R10" t="s">
+        <v>88</v>
+      </c>
+      <c r="S10" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="U10" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="R10" t="s">
-        <v>90</v>
-      </c>
-      <c r="S10" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="L11" t="s">
         <v>4</v>
       </c>
@@ -1478,28 +1472,28 @@
         <v>4</v>
       </c>
       <c r="N11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O11" t="s">
         <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tools to be featured
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/toolshed-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FE4AA-6CF1-964F-94D2-B8DFB383DE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718D6BD-0C4D-B847-AB75-E4B311E4562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>48</v>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="S6" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>60</v>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="S7" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>70</v>
@@ -1292,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="S8" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T8" t="s">
         <v>80</v>
@@ -1357,7 +1357,7 @@
         <v>88</v>
       </c>
       <c r="S9" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T9" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/Cookiesaurus/toolshed-app into test-aryan"
This reverts commit b02dcadcba95e4dfaccaf5bd1da5ee30080ed12a, reversing
changes made to 670a6904b83af8742955b326b9120926bad0ade8.
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718D6BD-0C4D-B847-AB75-E4B311E4562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FE4AA-6CF1-964F-94D2-B8DFB383DE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>48</v>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="S6" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>60</v>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="S7" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>70</v>
@@ -1292,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="S8" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="T8" t="s">
         <v>80</v>
@@ -1357,7 +1357,7 @@
         <v>88</v>
       </c>
       <c r="S9" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="T9" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Revert merge commit  237a1a
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/toolshed-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FE4AA-6CF1-964F-94D2-B8DFB383DE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718D6BD-0C4D-B847-AB75-E4B311E4562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="S5" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>48</v>
@@ -1162,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="S6" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>60</v>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="S7" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>70</v>
@@ -1292,7 +1292,7 @@
         <v>10</v>
       </c>
       <c r="S8" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T8" t="s">
         <v>80</v>
@@ -1357,7 +1357,7 @@
         <v>88</v>
       </c>
       <c r="S9" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="T9" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Added 25 more tools to the Excel sheet
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718D6BD-0C4D-B847-AB75-E4B311E4562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2908799-9C85-3E4B-AA45-D5CBCD2ED1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
+    <workbookView xWindow="41140" yWindow="-10480" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="253">
   <si>
     <t>I000240</t>
   </si>
@@ -356,13 +356,469 @@
   </si>
   <si>
     <t>Mobile Unit</t>
+  </si>
+  <si>
+    <t>B000001</t>
+  </si>
+  <si>
+    <t>Spray Paint Nozzle</t>
+  </si>
+  <si>
+    <t>RYOBI</t>
+  </si>
+  <si>
+    <t>Universal</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20220321_154300-970E6BF7-1004-37CA-5AE9-B2610C7750C4.jpg</t>
+  </si>
+  <si>
+    <t>36.99</t>
+  </si>
+  <si>
+    <t>Paint Nozzles</t>
+  </si>
+  <si>
+    <t>Painting, Pneumatic</t>
+  </si>
+  <si>
+    <t>B000002</t>
+  </si>
+  <si>
+    <t>Air Gun Nozzle</t>
+  </si>
+  <si>
+    <t>.5</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20220321_154253-238EBB32-D866-C22E-B127-4513A34E4D2F.jpg</t>
+  </si>
+  <si>
+    <t>Air Guns</t>
+  </si>
+  <si>
+    <t>Pneumatic, Automotive, Miscellaneous</t>
+  </si>
+  <si>
+    <t>B000003</t>
+  </si>
+  <si>
+    <t>Angle Die Grinder kit</t>
+  </si>
+  <si>
+    <t>Grizzly Industrial</t>
+  </si>
+  <si>
+    <t>2.55</t>
+  </si>
+  <si>
+    <t>Pneumatic powered, allows 1/8" and 1/4" shanks</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20220423_115122-97EDF4D4-E221-84A1-4FFA-51F1711215E8.jpg</t>
+  </si>
+  <si>
+    <t>57.95</t>
+  </si>
+  <si>
+    <t>Grinders</t>
+  </si>
+  <si>
+    <t>Pneumatic, Metalworking/Welding, Automotive</t>
+  </si>
+  <si>
+    <t>B000004</t>
+  </si>
+  <si>
+    <t>Air Gun Set</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>3 piece - 1/2" impact wrench, 3/8" ratchet wrench, 3/8" air hammer</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20220423_121622-703B07D5-8839-7A6A-AAC5-AFFE4264EA9B.jpg</t>
+  </si>
+  <si>
+    <t>99.88</t>
+  </si>
+  <si>
+    <t>B000005</t>
+  </si>
+  <si>
+    <t>6 Gal Air Compressor</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>6 gal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 PSI air Compressor 
+6 Gal. 
+</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/650755/image/20230816_154103-BE833ED9-1B9F-F9E0-B3C1-7FC54849CF41.jpg</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-attachments.s3-us-west-2.amazonaws.com/7/2147/item/650755/file_attachment/btfp02012-9C7FF8CC-1420-3AB4-9144-06B48EC50A5F.pdf</t>
+  </si>
+  <si>
+    <t>129.00</t>
+  </si>
+  <si>
+    <t>Compressors</t>
+  </si>
+  <si>
+    <t>Pneumatic, Carpentry/Woodworking, Roofing, Automotive</t>
+  </si>
+  <si>
+    <t>B000007</t>
+  </si>
+  <si>
+    <t>16 Gauge Finish Nailer</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>SB16 Fasteners</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/656910/image/20230928_132203-6B6F7A0B-9219-25E9-8DF1-CFAB91CF69A9.jpg</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-attachments.s3-us-west-2.amazonaws.com/7/2147/item/656910/file_attachment/sb150sx-7B2EF7E5-10F6-5BEF-FBB6-88C164EC0E99.pdf</t>
+  </si>
+  <si>
+    <t>131.01</t>
+  </si>
+  <si>
+    <t>Finish Nailers</t>
+  </si>
+  <si>
+    <t>B000008</t>
+  </si>
+  <si>
+    <t>Porter Cable</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>16 Gage Finish Nailer 
+takes 16 gage Brad nails 
+Fastener angle = STRAIGHT 
+Diameter 16 GAGE 
+Length 1" to 2-1/2" long ( 25-65MM)</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/672352/image/20220628_163818-38ADAECF-FCAB-F415-6794-8053D5050073.jpg</t>
+  </si>
+  <si>
+    <t>219.00</t>
+  </si>
+  <si>
+    <t>B000009</t>
+  </si>
+  <si>
+    <t>Cap Nailer</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>Comes with carrying case 
+Crown Staples</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20220701_172748-D11ECE40-73C6-F727-7985-178E08783973.jpg</t>
+  </si>
+  <si>
+    <t>107.62</t>
+  </si>
+  <si>
+    <t>Pneumatic, Roofing, Carpentry/Woodworking</t>
+  </si>
+  <si>
+    <t>B000010</t>
+  </si>
+  <si>
+    <t>6 Gallon Air Compressor</t>
+  </si>
+  <si>
+    <t>43.25</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/674186/image/20230928_132246-CCE46251-7D0B-F1BB-31E9-517A2A66FA77.jpg</t>
+  </si>
+  <si>
+    <t>273.99</t>
+  </si>
+  <si>
+    <t>B000011</t>
+  </si>
+  <si>
+    <t>Coil -fed Pneumatic Roofing Nailer</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Coil - Fed Pneumatic Roofing Nailer 
+with Case 
+takes 3/4" to 1-3/4" roofing nails</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/IMG_9249-92F4204D-8387-65F1-A693-19D040918411.jpg</t>
+  </si>
+  <si>
+    <t>229.00</t>
+  </si>
+  <si>
+    <t>Roofing Nailers</t>
+  </si>
+  <si>
+    <t>Roofing, Pneumatic</t>
+  </si>
+  <si>
+    <t>B000012</t>
+  </si>
+  <si>
+    <t>Coil-Fed Framing Nailer</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20221115_182838-901813BA-0F48-0B20-AAB8-D9C94C06BBFD.jpg</t>
+  </si>
+  <si>
+    <t>279.00</t>
+  </si>
+  <si>
+    <t>Framing Nailers</t>
+  </si>
+  <si>
+    <t>Pneumatic, Carpentry/Woodworking</t>
+  </si>
+  <si>
+    <t>B000013</t>
+  </si>
+  <si>
+    <t>21 Gauge Air Wire Stapler</t>
+  </si>
+  <si>
+    <t>HDC</t>
+  </si>
+  <si>
+    <t>Staple Sizes: 2 2/5" to 6 1/4" 
+60-120 PSI</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230124_134322-A711FACC-8A47-294F-692A-077213CFEB58.jpg</t>
+  </si>
+  <si>
+    <t>37.44</t>
+  </si>
+  <si>
+    <t>Staplers</t>
+  </si>
+  <si>
+    <t>Pneumatic, Crafting, Carpentry/Woodworking</t>
+  </si>
+  <si>
+    <t>B000014</t>
+  </si>
+  <si>
+    <t>18 Gauge Air Brad Nailer</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>18 Gage Pneumatic Brad Nailer with case 
+Takes 18 Gage Brads and takes lengths from 1-9/16" down to 13/32" 
+Requires an Air Compressor</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230214_145539-D5210C11-DFE0-A6F3-A247-927440C8816B.jpg</t>
+  </si>
+  <si>
+    <t>89.00</t>
+  </si>
+  <si>
+    <t>B000015</t>
+  </si>
+  <si>
+    <t>Crown Stapler</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>7/32" Staples</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230928_132207-508C327D-7994-EB26-78CF-B387B767B90B.jpg</t>
+  </si>
+  <si>
+    <t>109.99</t>
+  </si>
+  <si>
+    <t>Pneumatic, Carpentry/Woodworking, Flooring</t>
+  </si>
+  <si>
+    <t>J000245</t>
+  </si>
+  <si>
+    <t>Push Broom</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/IMG_9773%5B36%5D-F7FC9601-6340-597F-567E-99C95453F23E.jpg</t>
+  </si>
+  <si>
+    <t>22.97</t>
+  </si>
+  <si>
+    <t>Lawn Mowers</t>
+  </si>
+  <si>
+    <t>J000246</t>
+  </si>
+  <si>
+    <t>Grabber</t>
+  </si>
+  <si>
+    <t>48 in</t>
+  </si>
+  <si>
+    <t>to pick things up from high and low.</t>
+  </si>
+  <si>
+    <t>9.99</t>
+  </si>
+  <si>
+    <t>Hand Tools</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>J000247</t>
+  </si>
+  <si>
+    <t>Grabber for reaching items</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230324_172037-8BE5F1A5-DFAB-15F8-0D3C-E70555814A96.jpg</t>
+  </si>
+  <si>
+    <t>J000248</t>
+  </si>
+  <si>
+    <t>Hexagonal Crimping Tool</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Copper/Aluminum</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/767760/image/20230919_180956-5046BC10-7A6C-BF40-1FBD-0FC29DED3240.jpg</t>
+  </si>
+  <si>
+    <t>18.12</t>
+  </si>
+  <si>
+    <t>Crimpers</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>J000249</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230324_172037-1BC84E50-A5EE-12F9-74F0-E7DA712B4884.jpg</t>
+  </si>
+  <si>
+    <t>J000250</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230324_172037-EF363838-0967-01EE-6487-D36F631A9C2B.jpg</t>
+  </si>
+  <si>
+    <t>J000251</t>
+  </si>
+  <si>
+    <t>Receptical Circuit Tester</t>
+  </si>
+  <si>
+    <t>Commercial Electric</t>
+  </si>
+  <si>
+    <t>.25</t>
+  </si>
+  <si>
+    <t>Receptacle Circuit Tester ( plug in )</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/IMG_9605-6E1CD3D0-5C8B-EFE7-F600-D58E2C5EE731.jpg</t>
+  </si>
+  <si>
+    <t>24.00</t>
+  </si>
+  <si>
+    <t>Reciprocating Saws</t>
+  </si>
+  <si>
+    <t>Carpentry/Woodworking</t>
+  </si>
+  <si>
+    <t>J000252</t>
+  </si>
+  <si>
+    <t>J000253</t>
+  </si>
+  <si>
+    <t>Clamp &amp; Cut Edge Guide</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>50 in</t>
+  </si>
+  <si>
+    <t>https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230329_164430-5FC70911-E23D-FE6E-819F-26950F09F1DD.jpg</t>
+  </si>
+  <si>
+    <t>19.99</t>
+  </si>
+  <si>
+    <t>Clamps</t>
+  </si>
+  <si>
+    <t>Clamps/Vises, Carpentry/Woodworking, Metalworking/Welding, Miscellaneous</t>
+  </si>
+  <si>
+    <t>J000254</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -751,13 +1207,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="55" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
@@ -781,7 +1237,7 @@
     <col min="21" max="21" width="55.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -846,7 +1302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -911,7 +1367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -976,7 +1432,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="14" customHeight="1">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1041,7 +1497,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="14" customHeight="1">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1106,7 +1562,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1171,7 +1627,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1236,7 +1692,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1301,7 +1757,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1366,7 +1822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1431,7 +1887,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -1494,6 +1950,1696 @@
       </c>
       <c r="U11" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>110</v>
+      </c>
+      <c r="R12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" t="s">
+        <v>10</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>110</v>
+      </c>
+      <c r="R13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>125</v>
+      </c>
+      <c r="R14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14" t="s">
+        <v>10</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>133</v>
+      </c>
+      <c r="R15" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15" t="s">
+        <v>10</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="51">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>141</v>
+      </c>
+      <c r="R16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" t="s">
+        <v>10</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>150</v>
+      </c>
+      <c r="R17" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17" t="s">
+        <v>10</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="85">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>157</v>
+      </c>
+      <c r="R18" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="34">
+      <c r="A19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>163</v>
+      </c>
+      <c r="R19" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>169</v>
+      </c>
+      <c r="R20" t="s">
+        <v>10</v>
+      </c>
+      <c r="S20" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="51">
+      <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>175</v>
+      </c>
+      <c r="R21" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" t="s">
+        <v>3</v>
+      </c>
+      <c r="P22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>182</v>
+      </c>
+      <c r="R22" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="34">
+      <c r="A23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>190</v>
+      </c>
+      <c r="R23" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23" t="s">
+        <v>10</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="85">
+      <c r="A24" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>195</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="L24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" t="s">
+        <v>3</v>
+      </c>
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>198</v>
+      </c>
+      <c r="R24" t="s">
+        <v>10</v>
+      </c>
+      <c r="S24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>202</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="L25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>204</v>
+      </c>
+      <c r="R25" t="s">
+        <v>10</v>
+      </c>
+      <c r="S25" t="s">
+        <v>10</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" t="s">
+        <v>3</v>
+      </c>
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>59</v>
+      </c>
+      <c r="R26" t="s">
+        <v>10</v>
+      </c>
+      <c r="S26" t="s">
+        <v>10</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>69</v>
+      </c>
+      <c r="R27" t="s">
+        <v>10</v>
+      </c>
+      <c r="S27" t="s">
+        <v>10</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" t="s">
+        <v>207</v>
+      </c>
+      <c r="J28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" t="s">
+        <v>3</v>
+      </c>
+      <c r="P28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>210</v>
+      </c>
+      <c r="R28" t="s">
+        <v>10</v>
+      </c>
+      <c r="S28" t="s">
+        <v>10</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" t="s">
+        <v>215</v>
+      </c>
+      <c r="J29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>3</v>
+      </c>
+      <c r="P29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>216</v>
+      </c>
+      <c r="R29" t="s">
+        <v>10</v>
+      </c>
+      <c r="S29" t="s">
+        <v>10</v>
+      </c>
+      <c r="T29" t="s">
+        <v>217</v>
+      </c>
+      <c r="U29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" t="s">
+        <v>220</v>
+      </c>
+      <c r="J30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>216</v>
+      </c>
+      <c r="R30" t="s">
+        <v>10</v>
+      </c>
+      <c r="S30" t="s">
+        <v>10</v>
+      </c>
+      <c r="T30" t="s">
+        <v>217</v>
+      </c>
+      <c r="U30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>224</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>225</v>
+      </c>
+      <c r="J31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" t="s">
+        <v>3</v>
+      </c>
+      <c r="P31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>227</v>
+      </c>
+      <c r="R31" t="s">
+        <v>10</v>
+      </c>
+      <c r="S31" t="s">
+        <v>10</v>
+      </c>
+      <c r="T31" t="s">
+        <v>228</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" t="s">
+        <v>213</v>
+      </c>
+      <c r="J32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L32" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" t="s">
+        <v>3</v>
+      </c>
+      <c r="P32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>216</v>
+      </c>
+      <c r="R32" t="s">
+        <v>10</v>
+      </c>
+      <c r="S32" t="s">
+        <v>10</v>
+      </c>
+      <c r="T32" t="s">
+        <v>217</v>
+      </c>
+      <c r="U32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" t="s">
+        <v>213</v>
+      </c>
+      <c r="J33" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" t="s">
+        <v>4</v>
+      </c>
+      <c r="N33" t="s">
+        <v>4</v>
+      </c>
+      <c r="O33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P33" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>216</v>
+      </c>
+      <c r="R33" t="s">
+        <v>10</v>
+      </c>
+      <c r="S33" t="s">
+        <v>10</v>
+      </c>
+      <c r="T33" t="s">
+        <v>217</v>
+      </c>
+      <c r="U33" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B34" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D34" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" t="s">
+        <v>238</v>
+      </c>
+      <c r="J34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" t="s">
+        <v>3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>240</v>
+      </c>
+      <c r="R34" t="s">
+        <v>10</v>
+      </c>
+      <c r="S34" t="s">
+        <v>10</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" t="s">
+        <v>220</v>
+      </c>
+      <c r="J35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L35" t="s">
+        <v>4</v>
+      </c>
+      <c r="M35" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" t="s">
+        <v>4</v>
+      </c>
+      <c r="O35" t="s">
+        <v>3</v>
+      </c>
+      <c r="P35" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>216</v>
+      </c>
+      <c r="R35" t="s">
+        <v>10</v>
+      </c>
+      <c r="S35" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" t="s">
+        <v>217</v>
+      </c>
+      <c r="U35" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" t="s">
+        <v>244</v>
+      </c>
+      <c r="B36" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>247</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J36" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" t="s">
+        <v>3</v>
+      </c>
+      <c r="P36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>249</v>
+      </c>
+      <c r="R36" t="s">
+        <v>10</v>
+      </c>
+      <c r="S36" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" t="s">
+        <v>252</v>
+      </c>
+      <c r="B37" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>247</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J37" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L37" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" t="s">
+        <v>3</v>
+      </c>
+      <c r="P37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>249</v>
+      </c>
+      <c r="R37" t="s">
+        <v>10</v>
+      </c>
+      <c r="S37" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1510,6 +3656,33 @@
     <hyperlink ref="K9" r:id="rId9" xr:uid="{0BB4EAE0-5B23-684D-893C-28E2CDC17DCF}"/>
     <hyperlink ref="K10" r:id="rId10" xr:uid="{AA7B6BB3-60CF-C649-ADD2-0E92DFCA2B0C}"/>
     <hyperlink ref="K11" r:id="rId11" xr:uid="{BAF18D4F-672F-894D-BF70-9B5D5350363A}"/>
+    <hyperlink ref="K12" r:id="rId12" xr:uid="{274F1833-F6FB-0F4B-9C5D-7C28F89BC8CF}"/>
+    <hyperlink ref="K13" r:id="rId13" xr:uid="{3E151344-7101-D148-888F-7E40A20DE9CB}"/>
+    <hyperlink ref="K14" r:id="rId14" xr:uid="{8A2C67E7-9B08-FD47-B3D6-1F1880F4FA09}"/>
+    <hyperlink ref="K15" r:id="rId15" xr:uid="{212B3B24-2115-5D4D-B553-53BC47BA7F31}"/>
+    <hyperlink ref="L16" r:id="rId16" xr:uid="{C81E426F-F63D-C148-B48B-963B300FD889}"/>
+    <hyperlink ref="K16" r:id="rId17" xr:uid="{26B7ADAF-95A7-E54A-A1C2-6BA030E468C4}"/>
+    <hyperlink ref="L17" r:id="rId18" xr:uid="{334C5521-6CE3-4F43-8D5C-43294D2C01DF}"/>
+    <hyperlink ref="K17" r:id="rId19" xr:uid="{949B2736-8514-A04D-AF8E-BEDCABC1E47A}"/>
+    <hyperlink ref="K18" r:id="rId20" xr:uid="{BA887CD7-06D3-004C-8CC5-7587F2B90A2B}"/>
+    <hyperlink ref="K19" r:id="rId21" xr:uid="{E19365EE-04F9-7342-967C-F89F3F3D4993}"/>
+    <hyperlink ref="K20" r:id="rId22" xr:uid="{2B2D95EA-3755-D74B-ABD7-4A9D6DBFBACD}"/>
+    <hyperlink ref="K21" r:id="rId23" xr:uid="{341FE03C-F513-C14C-BC7D-21391FCA23C4}"/>
+    <hyperlink ref="K22" r:id="rId24" xr:uid="{AEA40714-1E00-F843-9DA0-F5EBD20A6B49}"/>
+    <hyperlink ref="K23" r:id="rId25" xr:uid="{C7308C2D-E26E-F446-BD8E-A6A07DA2A21E}"/>
+    <hyperlink ref="K24" r:id="rId26" xr:uid="{B2A94299-C5FF-514A-A4BE-74E1B9481E05}"/>
+    <hyperlink ref="K25" r:id="rId27" xr:uid="{158862B6-3B8A-3840-B560-A5AFFDAF8DA3}"/>
+    <hyperlink ref="K26" r:id="rId28" xr:uid="{4462CB88-6B7D-484B-AE7C-342B4DA42332}"/>
+    <hyperlink ref="K27" r:id="rId29" xr:uid="{C10798BA-DD5B-0340-87A9-C1AAD92DF738}"/>
+    <hyperlink ref="K34" r:id="rId30" xr:uid="{F1EDC946-D717-C845-BAAB-E975061B4F1E}"/>
+    <hyperlink ref="K30" r:id="rId31" xr:uid="{52011738-EF17-5442-B717-EBEC47E9B825}"/>
+    <hyperlink ref="K31" r:id="rId32" xr:uid="{3219D4A4-23F5-C049-AEF5-4C4B478317C5}"/>
+    <hyperlink ref="K32" r:id="rId33" xr:uid="{AAE751FB-DF68-5447-A383-F36645AB8732}"/>
+    <hyperlink ref="K33" r:id="rId34" xr:uid="{13855368-0811-4343-A8F2-C89AB0A20A36}"/>
+    <hyperlink ref="K35" r:id="rId35" xr:uid="{479E732E-B18A-EA4C-8090-34439E0B311E}"/>
+    <hyperlink ref="K36" r:id="rId36" xr:uid="{912B3CD0-4D35-3749-95C0-B62AF3DC4E5A}"/>
+    <hyperlink ref="K37" r:id="rId37" xr:uid="{2A86475C-D4A5-D24D-A988-033EA80B5C2E}"/>
+    <hyperlink ref="K28" r:id="rId38" xr:uid="{8C1287D5-B820-754A-92B9-3A142CC7BF64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removal of the states table, the addition of the genders table which adds both DOB and Gender back to accounts (This will need to be updated in the sign up form; It will probably be broken until this is changed), the change of the locations to include the specific mobile unit locations.
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5718D6BD-0C4D-B847-AB75-E4B311E4562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ECBF8A-E97B-CF47-8672-F212855C84ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="106">
   <si>
     <t>I000240</t>
   </si>
@@ -355,7 +355,10 @@
     <t>99.00</t>
   </si>
   <si>
-    <t>Mobile Unit</t>
+    <t>Mobile Unit - Thomas P. Ryan Center (Monday)</t>
+  </si>
+  <si>
+    <t>Mobile Unit - Edgerton Recreation Center (Tuesday)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,6 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,8 +768,8 @@
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -1383,10 +1387,10 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Allowed brand_name to be null
</commit_message>
<xml_diff>
--- a/Gate_Review_2_Tools.xlsx
+++ b/Gate_Review_2_Tools.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryceHofstrom/Senior Dev/501/toolshed-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iandinga/Desktop/Senior Dev/toolshed-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C145CD0E-E38D-5A46-97DC-9CBF82C29763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36AE5FC-C1B2-594B-B413-E8C06AE77599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{819443D6-F5FB-A94F-965C-46BF67CDAE2A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="270">
   <si>
     <t>I000240</t>
   </si>
@@ -734,9 +734,6 @@
   </si>
   <si>
     <t>Miscellaneous, Gardening/Landscape</t>
-  </si>
-  <si>
-    <t>noBrand</t>
   </si>
   <si>
     <t>20230322_141545-49E5A919-CDBF-4044-F465-E7F77739F08F.jpg</t>
@@ -963,27 +960,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1326,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1367,7 @@
         <v>22</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>23</v>
@@ -1459,7 +1436,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230322_141545-49E5A919-CDBF-4044-F465-E7F77739F08F.jpg</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M2" t="s">
         <v>4</v>
@@ -1528,7 +1505,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230919_152336-ED3ADFCF-DCC4-C14B-605D-D9E3CEE9426B.jpg</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M3" t="s">
         <v>4</v>
@@ -1597,7 +1574,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220322_110534-EAD31963-2BB0-7B76-7B7E-85614E41307F.jpg</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
@@ -1666,7 +1643,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220322_110042-43F676AE-7944-2301-1E30-8ED502D9F3BD.jpg</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M5" t="s">
         <v>4</v>
@@ -1735,7 +1712,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230928_132210-FE3BEB6D-E1F6-61E8-AC3F-B2FBAF564930.jpg</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M6" t="s">
         <v>4</v>
@@ -1804,7 +1781,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20231103_184220-72983043-87D3-79EE-063F-C0AA17ADA99A.jpg</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M7" t="s">
         <v>4</v>
@@ -1873,10 +1850,10 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/IMG_8837-D31E5BC0-E77D-D380-19E3-C35061A42D55.jpg</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N8" t="s">
         <v>4</v>
@@ -1923,10 +1900,10 @@
         <v>77</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
@@ -1942,7 +1919,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20231025_151806-F288637B-D1BB-EC9A-69DB-E5CB10BE23D4.jpg</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M9" t="s">
         <v>4</v>
@@ -1992,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -2011,7 +1988,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20240105_150058-F2F18019-C220-CCD6-00E4-715A4E9D6E3C.jpg</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M10" t="s">
         <v>4</v>
@@ -2080,7 +2057,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/IMG_0817-B1463399-007E-AF1D-C9AD-2C2309927C1D.jpg</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M11" t="s">
         <v>4</v>
@@ -2149,7 +2126,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220321_154300-970E6BF7-1004-37CA-5AE9-B2610C7750C4.jpg</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M12" t="s">
         <v>4</v>
@@ -2189,9 +2166,6 @@
       <c r="B13" t="s">
         <v>101</v>
       </c>
-      <c r="C13" t="s">
-        <v>227</v>
-      </c>
       <c r="D13" t="s">
         <v>102</v>
       </c>
@@ -2218,7 +2192,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220321_154253-238EBB32-D866-C22E-B127-4513A34E4D2F.jpg</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M13" t="s">
         <v>4</v>
@@ -2287,7 +2261,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220423_115122-97EDF4D4-E221-84A1-4FFA-51F1711215E8.jpg</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M14" t="s">
         <v>4</v>
@@ -2356,7 +2330,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220423_121622-703B07D5-8839-7A6A-AAC5-AFFE4264EA9B.jpg</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M15" t="s">
         <v>4</v>
@@ -2406,10 +2380,10 @@
         <v>121</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H16" t="s">
         <v>43</v>
@@ -2425,10 +2399,10 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230816_154103-BE833ED9-1B9F-F9E0-B3C1-7FC54849CF41.jpg</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N16" t="s">
         <v>4</v>
@@ -2475,10 +2449,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H17" t="s">
         <v>5</v>
@@ -2494,10 +2468,10 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230928_132203-6B6F7A0B-9219-25E9-8DF1-CFAB91CF69A9.jpg</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N17" t="s">
         <v>4</v>
@@ -2544,10 +2518,10 @@
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H18" t="s">
         <v>43</v>
@@ -2563,7 +2537,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220628_163818-38ADAECF-FCAB-F415-6794-8053D5050073.jpg</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M18" t="s">
         <v>4</v>
@@ -2632,7 +2606,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220701_172748-D11ECE40-73C6-F727-7985-178E08783973.jpg</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M19" t="s">
         <v>4</v>
@@ -2701,7 +2675,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230928_132246-CCE46251-7D0B-F1BB-31E9-517A2A66FA77.jpg</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M20" t="s">
         <v>4</v>
@@ -2770,7 +2744,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/IMG_9249-92F4204D-8387-65F1-A693-19D040918411.jpg</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M21" t="s">
         <v>4</v>
@@ -2839,7 +2813,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20221115_182838-901813BA-0F48-0B20-AAB8-D9C94C06BBFD.jpg</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M22" t="s">
         <v>4</v>
@@ -2908,7 +2882,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230124_134322-A711FACC-8A47-294F-692A-077213CFEB58.jpg</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M23" t="s">
         <v>4</v>
@@ -2948,9 +2922,6 @@
       <c r="B24" t="s">
         <v>168</v>
       </c>
-      <c r="C24" t="s">
-        <v>227</v>
-      </c>
       <c r="D24" t="s">
         <v>169</v>
       </c>
@@ -2977,7 +2948,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230214_145539-D5210C11-DFE0-A6F3-A247-927440C8816B.jpg</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M24" t="s">
         <v>4</v>
@@ -3046,7 +3017,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230928_132207-508C327D-7994-EB26-78CF-B387B767B90B.jpg</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M25" t="s">
         <v>4</v>
@@ -3086,9 +3057,6 @@
       <c r="B26" t="s">
         <v>179</v>
       </c>
-      <c r="C26" t="s">
-        <v>227</v>
-      </c>
       <c r="D26" t="s">
         <v>180</v>
       </c>
@@ -3111,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M26" t="s">
         <v>4</v>
@@ -3154,9 +3122,6 @@
       <c r="B27" t="s">
         <v>183</v>
       </c>
-      <c r="C27" t="s">
-        <v>227</v>
-      </c>
       <c r="D27" t="s">
         <v>102</v>
       </c>
@@ -3183,7 +3148,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230324_172037-8BE5F1A5-DFAB-15F8-0D3C-E70555814A96.jpg</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M27" t="s">
         <v>4</v>
@@ -3223,9 +3188,6 @@
       <c r="B28" t="s">
         <v>190</v>
       </c>
-      <c r="C28" t="s">
-        <v>227</v>
-      </c>
       <c r="D28" t="s">
         <v>191</v>
       </c>
@@ -3252,7 +3214,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230919_180956-5046BC10-7A6C-BF40-1FBD-0FC29DED3240.jpg</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M28" t="s">
         <v>4</v>
@@ -3292,9 +3254,6 @@
       <c r="B29" t="s">
         <v>183</v>
       </c>
-      <c r="C29" t="s">
-        <v>227</v>
-      </c>
       <c r="D29" t="s">
         <v>102</v>
       </c>
@@ -3321,7 +3280,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230324_172037-1BC84E50-A5EE-12F9-74F0-E7DA712B4884.jpg</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M29" t="s">
         <v>4</v>
@@ -3361,9 +3320,6 @@
       <c r="B30" t="s">
         <v>183</v>
       </c>
-      <c r="C30" t="s">
-        <v>227</v>
-      </c>
       <c r="D30" t="s">
         <v>102</v>
       </c>
@@ -3390,7 +3346,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230324_172037-EF363838-0967-01EE-6487-D36F631A9C2B.jpg</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M30" t="s">
         <v>4</v>
@@ -3459,7 +3415,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/IMG_9605-6E1CD3D0-5C8B-EFE7-F600-D58E2C5EE731.jpg</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M31" t="s">
         <v>4</v>
@@ -3499,9 +3455,6 @@
       <c r="B32" t="s">
         <v>183</v>
       </c>
-      <c r="C32" t="s">
-        <v>227</v>
-      </c>
       <c r="D32" t="s">
         <v>102</v>
       </c>
@@ -3528,7 +3481,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230324_172037-8BE5F1A5-DFAB-15F8-0D3C-E70555814A96.jpg</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M32" t="s">
         <v>4</v>
@@ -3597,7 +3550,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230329_164430-5FC70911-E23D-FE6E-819F-26950F09F1DD.jpg</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M33" t="s">
         <v>4</v>
@@ -3666,7 +3619,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230329_164430-5FC70911-E23D-FE6E-819F-26950F09F1DD.jpg</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M34" t="s">
         <v>4</v>
@@ -3735,7 +3688,7 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20220524_180142-C16A38EF-BD61-60F6-5649-A714B97F93D3.jpg</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M35" s="6"/>
       <c r="N35" t="s">
@@ -3802,10 +3755,10 @@
         <v>https://seachtoolshedimages.s3.us-east-2.amazonaws.com/20230802_170739-5ABB452A-8F78-7FAD-DE92-40F4DD2E88E7.jpg</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N36" t="s">
         <v>4</v>
@@ -3838,7 +3791,7 @@
   </sheetData>
   <autoFilter ref="A1:V11" xr:uid="{01F1CD99-5819-CF45-B46D-1DBA696BD75C}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="L36" r:id="rId1" display="https://myturn-prod-images-in.s3-us-west-2.amazonaws.com/7/2147/item/---/image/20230802_170739-5ABB452A-8F78-7FAD-DE92-40F4DD2E88E7.jpg" xr:uid="{A17B5CBB-5BAF-B943-ABA6-B75ED752F9DD}"/>

</xml_diff>